<commit_message>
Created one library per derived sample of source sample, accepted empty concentration for DNA libraries
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Library_conversion_v3_9_0.xlsx
+++ b/backend/fms_core/static/submission_templates/Library_conversion_v3_9_0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sballesteros/Documents/Freezeman/freezeman/backend/fms_core/static/submission_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F93F0052-632C-714E-9DE5-E7CC671D48EE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9D8C803-D536-9440-9461-5EE900AAEA6E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15940" xr2:uid="{405E7239-1D14-6F47-A693-F6EDB1481B97}"/>
+    <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15940" activeTab="1" xr2:uid="{405E7239-1D14-6F47-A693-F6EDB1481B97}"/>
   </bookViews>
   <sheets>
     <sheet name="Conversion Batch" sheetId="1" r:id="rId1"/>
@@ -826,7 +826,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DBEF91C-DC9D-184F-9DE0-D7E7DAC2E4DD}">
   <dimension ref="A1:AMG387"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2997,7 +2997,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D07BE83E-81BB-7B4B-B20C-1C27C9CCE468}">
   <dimension ref="A1:O484"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>

<commit_message>
Fixed the conversion template
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Library_conversion_v3_9_0.xlsx
+++ b/backend/fms_core/static/submission_templates/Library_conversion_v3_9_0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sballesteros/Documents/Freezeman/freezeman/backend/fms_core/static/submission_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9D8C803-D536-9440-9461-5EE900AAEA6E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42543C5E-7D8F-294B-B53A-2A43377C2677}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15940" activeTab="1" xr2:uid="{405E7239-1D14-6F47-A693-F6EDB1481B97}"/>
+    <workbookView xWindow="780" yWindow="980" windowWidth="27640" windowHeight="15940" xr2:uid="{405E7239-1D14-6F47-A693-F6EDB1481B97}"/>
   </bookViews>
   <sheets>
     <sheet name="Conversion Batch" sheetId="1" r:id="rId1"/>
@@ -275,10 +275,10 @@
     <t>MGI_Conversion_AppC</t>
   </si>
   <si>
-    <t>Library Technician Name</t>
+    <t>Kit Used</t>
   </si>
   <si>
-    <t>Library Kit Lot</t>
+    <t>Kit Lot</t>
   </si>
 </sst>
 </file>
@@ -504,7 +504,7 @@
       <sheetName val="Index"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
+      <sheetData sheetId="0" refreshError="1"/>
       <sheetData sheetId="1" refreshError="1"/>
       <sheetData sheetId="2"/>
     </sheetDataSet>
@@ -826,7 +826,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DBEF91C-DC9D-184F-9DE0-D7E7DAC2E4DD}">
   <dimension ref="A1:AMG387"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -930,10 +930,10 @@
         <v>6</v>
       </c>
       <c r="E10" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="35" t="s">
         <v>60</v>
-      </c>
-      <c r="F10" s="35" t="s">
-        <v>7</v>
       </c>
       <c r="G10" s="35" t="s">
         <v>61</v>
@@ -1175,7 +1175,6 @@
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="5"/>
       <c r="B48" s="13"/>
-      <c r="C48" s="13"/>
       <c r="D48" s="13"/>
       <c r="E48" s="12"/>
       <c r="F48" s="1"/>
@@ -1183,7 +1182,6 @@
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="5"/>
       <c r="B49" s="13"/>
-      <c r="C49" s="13"/>
       <c r="D49" s="13"/>
       <c r="E49" s="12"/>
       <c r="F49" s="1"/>
@@ -1191,7 +1189,6 @@
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="5"/>
       <c r="B50" s="13"/>
-      <c r="C50" s="13"/>
       <c r="D50" s="13"/>
       <c r="E50" s="12"/>
       <c r="F50" s="1"/>
@@ -1199,7 +1196,6 @@
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="5"/>
       <c r="B51" s="13"/>
-      <c r="C51" s="13"/>
       <c r="D51" s="13"/>
       <c r="E51" s="12"/>
       <c r="F51" s="1"/>
@@ -1207,7 +1203,6 @@
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="5"/>
       <c r="B52" s="13"/>
-      <c r="C52" s="13"/>
       <c r="D52" s="13"/>
       <c r="E52" s="12"/>
       <c r="F52" s="1"/>
@@ -1215,7 +1210,6 @@
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="5"/>
       <c r="B53" s="13"/>
-      <c r="C53" s="13"/>
       <c r="D53" s="13"/>
       <c r="E53" s="12"/>
       <c r="F53" s="1"/>
@@ -1223,7 +1217,6 @@
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="5"/>
       <c r="B54" s="13"/>
-      <c r="C54" s="13"/>
       <c r="D54" s="13"/>
       <c r="E54" s="12"/>
       <c r="F54" s="1"/>
@@ -1231,7 +1224,6 @@
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="5"/>
       <c r="B55" s="13"/>
-      <c r="C55" s="13"/>
       <c r="D55" s="13"/>
       <c r="E55" s="12"/>
       <c r="F55" s="1"/>
@@ -1239,7 +1231,6 @@
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="5"/>
       <c r="B56" s="13"/>
-      <c r="C56" s="13"/>
       <c r="D56" s="13"/>
       <c r="E56" s="12"/>
       <c r="F56" s="1"/>
@@ -1247,7 +1238,6 @@
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="5"/>
       <c r="B57" s="13"/>
-      <c r="C57" s="13"/>
       <c r="D57" s="13"/>
       <c r="E57" s="12"/>
       <c r="F57" s="1"/>
@@ -1255,7 +1245,6 @@
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="5"/>
       <c r="B58" s="13"/>
-      <c r="C58" s="13"/>
       <c r="D58" s="13"/>
       <c r="E58" s="12"/>
       <c r="F58" s="1"/>
@@ -1263,7 +1252,6 @@
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="5"/>
       <c r="B59" s="13"/>
-      <c r="C59" s="13"/>
       <c r="D59" s="13"/>
       <c r="E59" s="12"/>
       <c r="F59" s="1"/>
@@ -1271,7 +1259,6 @@
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="5"/>
       <c r="B60" s="13"/>
-      <c r="C60" s="13"/>
       <c r="D60" s="13"/>
       <c r="E60" s="12"/>
       <c r="F60" s="1"/>
@@ -1279,7 +1266,6 @@
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="5"/>
       <c r="B61" s="13"/>
-      <c r="C61" s="13"/>
       <c r="D61" s="13"/>
       <c r="E61" s="12"/>
       <c r="F61" s="1"/>
@@ -1287,7 +1273,6 @@
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="5"/>
       <c r="B62" s="13"/>
-      <c r="C62" s="13"/>
       <c r="D62" s="13"/>
       <c r="E62" s="12"/>
       <c r="F62" s="1"/>
@@ -1295,7 +1280,6 @@
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="5"/>
       <c r="B63" s="13"/>
-      <c r="C63" s="13"/>
       <c r="D63" s="13"/>
       <c r="E63" s="12"/>
       <c r="F63" s="1"/>
@@ -1303,7 +1287,6 @@
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="5"/>
       <c r="B64" s="13"/>
-      <c r="C64" s="13"/>
       <c r="D64" s="13"/>
       <c r="E64" s="12"/>
       <c r="F64" s="1"/>
@@ -1311,7 +1294,6 @@
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="5"/>
       <c r="B65" s="13"/>
-      <c r="C65" s="13"/>
       <c r="D65" s="13"/>
       <c r="E65" s="12"/>
       <c r="F65" s="1"/>
@@ -1319,7 +1301,6 @@
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" s="5"/>
       <c r="B66" s="13"/>
-      <c r="C66" s="13"/>
       <c r="D66" s="13"/>
       <c r="E66" s="12"/>
       <c r="F66" s="1"/>
@@ -1327,7 +1308,6 @@
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="5"/>
       <c r="B67" s="13"/>
-      <c r="C67" s="13"/>
       <c r="D67" s="13"/>
       <c r="E67" s="12"/>
       <c r="F67" s="1"/>
@@ -1335,7 +1315,6 @@
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" s="5"/>
       <c r="B68" s="13"/>
-      <c r="C68" s="13"/>
       <c r="D68" s="13"/>
       <c r="E68" s="12"/>
       <c r="F68" s="1"/>
@@ -1343,7 +1322,6 @@
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" s="5"/>
       <c r="B69" s="13"/>
-      <c r="C69" s="13"/>
       <c r="D69" s="13"/>
       <c r="E69" s="12"/>
       <c r="F69" s="1"/>
@@ -1351,7 +1329,6 @@
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" s="5"/>
       <c r="B70" s="13"/>
-      <c r="C70" s="13"/>
       <c r="D70" s="13"/>
       <c r="E70" s="12"/>
       <c r="F70" s="1"/>
@@ -1359,7 +1336,6 @@
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" s="5"/>
       <c r="B71" s="13"/>
-      <c r="C71" s="13"/>
       <c r="D71" s="13"/>
       <c r="E71" s="12"/>
       <c r="F71" s="1"/>
@@ -1367,7 +1343,6 @@
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" s="5"/>
       <c r="B72" s="13"/>
-      <c r="C72" s="13"/>
       <c r="D72" s="13"/>
       <c r="E72" s="12"/>
       <c r="F72" s="1"/>
@@ -1375,7 +1350,6 @@
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" s="5"/>
       <c r="B73" s="13"/>
-      <c r="C73" s="13"/>
       <c r="D73" s="13"/>
       <c r="E73" s="12"/>
       <c r="F73" s="1"/>
@@ -1383,7 +1357,6 @@
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" s="5"/>
       <c r="B74" s="13"/>
-      <c r="C74" s="13"/>
       <c r="D74" s="13"/>
       <c r="E74" s="12"/>
       <c r="F74" s="1"/>
@@ -1391,7 +1364,6 @@
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" s="5"/>
       <c r="B75" s="13"/>
-      <c r="C75" s="13"/>
       <c r="D75" s="13"/>
       <c r="E75" s="12"/>
       <c r="F75" s="1"/>
@@ -1399,7 +1371,6 @@
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" s="5"/>
       <c r="B76" s="13"/>
-      <c r="C76" s="13"/>
       <c r="D76" s="13"/>
       <c r="E76" s="12"/>
       <c r="F76" s="1"/>
@@ -1407,7 +1378,6 @@
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" s="5"/>
       <c r="B77" s="13"/>
-      <c r="C77" s="13"/>
       <c r="D77" s="13"/>
       <c r="E77" s="12"/>
       <c r="F77" s="1"/>
@@ -1415,7 +1385,6 @@
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" s="5"/>
       <c r="B78" s="13"/>
-      <c r="C78" s="13"/>
       <c r="D78" s="13"/>
       <c r="E78" s="12"/>
       <c r="F78" s="1"/>
@@ -1423,7 +1392,6 @@
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" s="5"/>
       <c r="B79" s="13"/>
-      <c r="C79" s="13"/>
       <c r="D79" s="13"/>
       <c r="E79" s="12"/>
       <c r="F79" s="1"/>
@@ -1431,7 +1399,6 @@
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" s="5"/>
       <c r="B80" s="13"/>
-      <c r="C80" s="13"/>
       <c r="D80" s="13"/>
       <c r="E80" s="12"/>
       <c r="F80" s="1"/>
@@ -1439,7 +1406,6 @@
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" s="5"/>
       <c r="B81" s="13"/>
-      <c r="C81" s="13"/>
       <c r="D81" s="13"/>
       <c r="E81" s="12"/>
       <c r="F81" s="1"/>
@@ -1447,7 +1413,6 @@
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" s="5"/>
       <c r="B82" s="13"/>
-      <c r="C82" s="13"/>
       <c r="D82" s="13"/>
       <c r="E82" s="12"/>
       <c r="F82" s="1"/>
@@ -1455,7 +1420,6 @@
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" s="5"/>
       <c r="B83" s="13"/>
-      <c r="C83" s="13"/>
       <c r="D83" s="13"/>
       <c r="E83" s="12"/>
       <c r="F83" s="1"/>
@@ -1463,7 +1427,6 @@
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" s="5"/>
       <c r="B84" s="13"/>
-      <c r="C84" s="13"/>
       <c r="D84" s="13"/>
       <c r="E84" s="12"/>
       <c r="F84" s="1"/>
@@ -1471,7 +1434,6 @@
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" s="5"/>
       <c r="B85" s="13"/>
-      <c r="C85" s="13"/>
       <c r="D85" s="13"/>
       <c r="E85" s="12"/>
       <c r="F85" s="1"/>
@@ -1479,7 +1441,6 @@
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" s="5"/>
       <c r="B86" s="13"/>
-      <c r="C86" s="13"/>
       <c r="D86" s="13"/>
       <c r="E86" s="12"/>
       <c r="F86" s="1"/>
@@ -1487,7 +1448,6 @@
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" s="5"/>
       <c r="B87" s="13"/>
-      <c r="C87" s="13"/>
       <c r="D87" s="13"/>
       <c r="E87" s="12"/>
       <c r="F87" s="1"/>
@@ -1495,7 +1455,6 @@
     <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" s="5"/>
       <c r="B88" s="13"/>
-      <c r="C88" s="13"/>
       <c r="D88" s="13"/>
       <c r="E88" s="12"/>
       <c r="F88" s="1"/>
@@ -1503,7 +1462,6 @@
     <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" s="5"/>
       <c r="B89" s="13"/>
-      <c r="C89" s="13"/>
       <c r="D89" s="13"/>
       <c r="E89" s="12"/>
       <c r="F89" s="1"/>
@@ -1511,7 +1469,6 @@
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" s="5"/>
       <c r="B90" s="13"/>
-      <c r="C90" s="13"/>
       <c r="D90" s="13"/>
       <c r="E90" s="12"/>
       <c r="F90" s="1"/>
@@ -1519,7 +1476,6 @@
     <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" s="5"/>
       <c r="B91" s="13"/>
-      <c r="C91" s="13"/>
       <c r="D91" s="13"/>
       <c r="E91" s="12"/>
       <c r="F91" s="1"/>
@@ -1527,7 +1483,6 @@
     <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" s="5"/>
       <c r="B92" s="13"/>
-      <c r="C92" s="13"/>
       <c r="D92" s="13"/>
       <c r="E92" s="12"/>
       <c r="F92" s="1"/>
@@ -1535,7 +1490,6 @@
     <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" s="5"/>
       <c r="B93" s="13"/>
-      <c r="C93" s="13"/>
       <c r="D93" s="13"/>
       <c r="E93" s="12"/>
       <c r="F93" s="1"/>
@@ -1543,7 +1497,6 @@
     <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" s="5"/>
       <c r="B94" s="13"/>
-      <c r="C94" s="13"/>
       <c r="D94" s="13"/>
       <c r="E94" s="12"/>
       <c r="F94" s="1"/>
@@ -1551,532 +1504,456 @@
     <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" s="5"/>
       <c r="B95" s="13"/>
-      <c r="C95" s="13"/>
       <c r="D95" s="13"/>
       <c r="E95" s="12"/>
       <c r="F95" s="1"/>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B96" s="13"/>
-      <c r="C96" s="13"/>
       <c r="D96" s="13"/>
       <c r="E96" s="12"/>
       <c r="F96" s="1"/>
     </row>
     <row r="97" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B97" s="13"/>
-      <c r="C97" s="13"/>
       <c r="D97" s="13"/>
       <c r="E97" s="12"/>
       <c r="F97" s="1"/>
     </row>
     <row r="98" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B98" s="13"/>
-      <c r="C98" s="13"/>
       <c r="D98" s="13"/>
       <c r="E98" s="12"/>
       <c r="F98" s="1"/>
     </row>
     <row r="99" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B99" s="13"/>
-      <c r="C99" s="13"/>
       <c r="D99" s="13"/>
       <c r="E99" s="12"/>
       <c r="F99" s="1"/>
     </row>
     <row r="100" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B100" s="13"/>
-      <c r="C100" s="13"/>
       <c r="D100" s="13"/>
       <c r="E100" s="12"/>
       <c r="F100" s="1"/>
     </row>
     <row r="101" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B101" s="13"/>
-      <c r="C101" s="13"/>
       <c r="D101" s="13"/>
       <c r="E101" s="12"/>
       <c r="F101" s="1"/>
     </row>
     <row r="102" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B102" s="13"/>
-      <c r="C102" s="13"/>
       <c r="D102" s="13"/>
       <c r="E102" s="12"/>
       <c r="F102" s="1"/>
     </row>
     <row r="103" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B103" s="13"/>
-      <c r="C103" s="13"/>
       <c r="D103" s="13"/>
       <c r="E103" s="12"/>
       <c r="F103" s="1"/>
     </row>
     <row r="104" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B104" s="13"/>
-      <c r="C104" s="13"/>
       <c r="D104" s="13"/>
       <c r="E104" s="12"/>
       <c r="F104" s="1"/>
     </row>
     <row r="105" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B105" s="13"/>
-      <c r="C105" s="13"/>
       <c r="D105" s="13"/>
       <c r="E105" s="12"/>
       <c r="F105" s="1"/>
     </row>
     <row r="106" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B106" s="13"/>
-      <c r="C106" s="13"/>
       <c r="D106" s="13"/>
       <c r="E106" s="12"/>
       <c r="F106" s="1"/>
     </row>
     <row r="107" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B107" s="13"/>
-      <c r="C107" s="13"/>
       <c r="D107" s="13"/>
       <c r="E107" s="12"/>
       <c r="F107" s="1"/>
     </row>
     <row r="108" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B108" s="13"/>
-      <c r="C108" s="13"/>
       <c r="D108" s="13"/>
       <c r="E108" s="12"/>
       <c r="F108" s="1"/>
     </row>
     <row r="109" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B109" s="13"/>
-      <c r="C109" s="13"/>
       <c r="D109" s="13"/>
       <c r="E109" s="12"/>
       <c r="F109" s="1"/>
     </row>
     <row r="110" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B110" s="13"/>
-      <c r="C110" s="13"/>
       <c r="D110" s="13"/>
       <c r="E110" s="12"/>
       <c r="F110" s="1"/>
     </row>
     <row r="111" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B111" s="13"/>
-      <c r="C111" s="13"/>
       <c r="D111" s="13"/>
       <c r="E111" s="12"/>
       <c r="F111" s="1"/>
     </row>
     <row r="112" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B112" s="13"/>
-      <c r="C112" s="13"/>
       <c r="D112" s="13"/>
       <c r="E112" s="12"/>
       <c r="F112" s="1"/>
     </row>
     <row r="113" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B113" s="13"/>
-      <c r="C113" s="13"/>
       <c r="D113" s="13"/>
       <c r="E113" s="12"/>
       <c r="F113" s="1"/>
     </row>
     <row r="114" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B114" s="13"/>
-      <c r="C114" s="13"/>
       <c r="D114" s="13"/>
       <c r="E114" s="12"/>
       <c r="F114" s="1"/>
     </row>
     <row r="115" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B115" s="13"/>
-      <c r="C115" s="13"/>
       <c r="D115" s="13"/>
       <c r="E115" s="12"/>
       <c r="F115" s="1"/>
     </row>
     <row r="116" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B116" s="13"/>
-      <c r="C116" s="13"/>
       <c r="D116" s="13"/>
       <c r="E116" s="12"/>
       <c r="F116" s="1"/>
     </row>
     <row r="117" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B117" s="13"/>
-      <c r="C117" s="13"/>
       <c r="D117" s="13"/>
       <c r="E117" s="12"/>
       <c r="F117" s="1"/>
     </row>
     <row r="118" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B118" s="13"/>
-      <c r="C118" s="13"/>
       <c r="D118" s="13"/>
       <c r="E118" s="12"/>
       <c r="F118" s="1"/>
     </row>
     <row r="119" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B119" s="13"/>
-      <c r="C119" s="13"/>
       <c r="D119" s="13"/>
       <c r="E119" s="12"/>
       <c r="F119" s="1"/>
     </row>
     <row r="120" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B120" s="13"/>
-      <c r="C120" s="13"/>
       <c r="D120" s="13"/>
       <c r="E120" s="12"/>
       <c r="F120" s="1"/>
     </row>
     <row r="121" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B121" s="13"/>
-      <c r="C121" s="13"/>
       <c r="D121" s="13"/>
       <c r="E121" s="12"/>
       <c r="F121" s="1"/>
     </row>
     <row r="122" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B122" s="13"/>
-      <c r="C122" s="13"/>
       <c r="D122" s="13"/>
       <c r="E122" s="12"/>
       <c r="F122" s="1"/>
     </row>
     <row r="123" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B123" s="13"/>
-      <c r="C123" s="13"/>
       <c r="D123" s="13"/>
       <c r="E123" s="12"/>
       <c r="F123" s="1"/>
     </row>
     <row r="124" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B124" s="13"/>
-      <c r="C124" s="13"/>
       <c r="D124" s="13"/>
       <c r="E124" s="12"/>
       <c r="F124" s="1"/>
     </row>
     <row r="125" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B125" s="13"/>
-      <c r="C125" s="13"/>
       <c r="D125" s="13"/>
       <c r="E125" s="12"/>
       <c r="F125" s="1"/>
     </row>
     <row r="126" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B126" s="13"/>
-      <c r="C126" s="13"/>
       <c r="D126" s="13"/>
       <c r="E126" s="12"/>
       <c r="F126" s="1"/>
     </row>
     <row r="127" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B127" s="13"/>
-      <c r="C127" s="13"/>
       <c r="D127" s="13"/>
       <c r="E127" s="12"/>
       <c r="F127" s="1"/>
     </row>
     <row r="128" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B128" s="13"/>
-      <c r="C128" s="13"/>
       <c r="D128" s="13"/>
       <c r="E128" s="12"/>
       <c r="F128" s="1"/>
     </row>
     <row r="129" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B129" s="13"/>
-      <c r="C129" s="13"/>
       <c r="D129" s="13"/>
       <c r="E129" s="12"/>
       <c r="F129" s="1"/>
     </row>
     <row r="130" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B130" s="13"/>
-      <c r="C130" s="13"/>
       <c r="D130" s="13"/>
       <c r="E130" s="12"/>
       <c r="F130" s="1"/>
     </row>
     <row r="131" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B131" s="13"/>
-      <c r="C131" s="13"/>
       <c r="D131" s="13"/>
       <c r="E131" s="12"/>
       <c r="F131" s="1"/>
     </row>
     <row r="132" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B132" s="13"/>
-      <c r="C132" s="13"/>
       <c r="D132" s="13"/>
       <c r="E132" s="12"/>
       <c r="F132" s="1"/>
     </row>
     <row r="133" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B133" s="13"/>
-      <c r="C133" s="13"/>
       <c r="D133" s="13"/>
       <c r="E133" s="12"/>
       <c r="F133" s="1"/>
     </row>
     <row r="134" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B134" s="13"/>
-      <c r="C134" s="13"/>
       <c r="D134" s="13"/>
       <c r="E134" s="12"/>
       <c r="F134" s="1"/>
     </row>
     <row r="135" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B135" s="13"/>
-      <c r="C135" s="13"/>
       <c r="D135" s="13"/>
       <c r="E135" s="12"/>
       <c r="F135" s="1"/>
     </row>
     <row r="136" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B136" s="13"/>
-      <c r="C136" s="13"/>
       <c r="D136" s="13"/>
       <c r="E136" s="12"/>
       <c r="F136" s="1"/>
     </row>
     <row r="137" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B137" s="13"/>
-      <c r="C137" s="13"/>
       <c r="D137" s="13"/>
       <c r="E137" s="12"/>
       <c r="F137" s="1"/>
     </row>
     <row r="138" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B138" s="13"/>
-      <c r="C138" s="13"/>
       <c r="D138" s="13"/>
       <c r="E138" s="12"/>
       <c r="F138" s="1"/>
     </row>
     <row r="139" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B139" s="13"/>
-      <c r="C139" s="13"/>
       <c r="D139" s="13"/>
       <c r="E139" s="12"/>
       <c r="F139" s="1"/>
     </row>
     <row r="140" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B140" s="13"/>
-      <c r="C140" s="13"/>
       <c r="D140" s="13"/>
       <c r="E140" s="12"/>
       <c r="F140" s="1"/>
     </row>
     <row r="141" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B141" s="13"/>
-      <c r="C141" s="13"/>
       <c r="D141" s="13"/>
       <c r="E141" s="12"/>
       <c r="F141" s="1"/>
     </row>
     <row r="142" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B142" s="13"/>
-      <c r="C142" s="13"/>
       <c r="D142" s="13"/>
       <c r="E142" s="12"/>
       <c r="F142" s="1"/>
     </row>
     <row r="143" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B143" s="13"/>
-      <c r="C143" s="13"/>
       <c r="D143" s="13"/>
       <c r="E143" s="12"/>
       <c r="F143" s="1"/>
     </row>
     <row r="144" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B144" s="13"/>
-      <c r="C144" s="13"/>
       <c r="D144" s="13"/>
       <c r="E144" s="12"/>
       <c r="F144" s="1"/>
     </row>
     <row r="145" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B145" s="13"/>
-      <c r="C145" s="13"/>
       <c r="D145" s="13"/>
       <c r="E145" s="12"/>
       <c r="F145" s="1"/>
     </row>
     <row r="146" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B146" s="13"/>
-      <c r="C146" s="13"/>
       <c r="D146" s="13"/>
       <c r="E146" s="12"/>
       <c r="F146" s="1"/>
     </row>
     <row r="147" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B147" s="13"/>
-      <c r="C147" s="13"/>
       <c r="D147" s="13"/>
       <c r="E147" s="12"/>
       <c r="F147" s="1"/>
     </row>
     <row r="148" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B148" s="13"/>
-      <c r="C148" s="13"/>
       <c r="D148" s="13"/>
       <c r="E148" s="12"/>
       <c r="F148" s="1"/>
     </row>
     <row r="149" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B149" s="13"/>
-      <c r="C149" s="13"/>
       <c r="D149" s="13"/>
       <c r="E149" s="12"/>
       <c r="F149" s="1"/>
     </row>
     <row r="150" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B150" s="13"/>
-      <c r="C150" s="13"/>
       <c r="D150" s="13"/>
       <c r="E150" s="12"/>
       <c r="F150" s="1"/>
     </row>
     <row r="151" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B151" s="13"/>
-      <c r="C151" s="13"/>
       <c r="D151" s="13"/>
       <c r="E151" s="12"/>
       <c r="F151" s="1"/>
     </row>
     <row r="152" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B152" s="13"/>
-      <c r="C152" s="13"/>
       <c r="D152" s="13"/>
       <c r="E152" s="12"/>
       <c r="F152" s="1"/>
     </row>
     <row r="153" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B153" s="13"/>
-      <c r="C153" s="13"/>
       <c r="D153" s="13"/>
       <c r="E153" s="12"/>
       <c r="F153" s="1"/>
     </row>
     <row r="154" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B154" s="13"/>
-      <c r="C154" s="13"/>
       <c r="D154" s="13"/>
       <c r="E154" s="12"/>
       <c r="F154" s="1"/>
     </row>
     <row r="155" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B155" s="13"/>
-      <c r="C155" s="13"/>
       <c r="D155" s="13"/>
       <c r="E155" s="12"/>
       <c r="F155" s="1"/>
     </row>
     <row r="156" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B156" s="13"/>
-      <c r="C156" s="13"/>
       <c r="D156" s="13"/>
       <c r="E156" s="12"/>
       <c r="F156" s="1"/>
     </row>
     <row r="157" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B157" s="13"/>
-      <c r="C157" s="13"/>
       <c r="D157" s="13"/>
       <c r="E157" s="12"/>
       <c r="F157" s="1"/>
     </row>
     <row r="158" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B158" s="13"/>
-      <c r="C158" s="13"/>
       <c r="D158" s="13"/>
       <c r="E158" s="12"/>
       <c r="F158" s="1"/>
     </row>
     <row r="159" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B159" s="13"/>
-      <c r="C159" s="13"/>
       <c r="D159" s="13"/>
       <c r="E159" s="12"/>
       <c r="F159" s="1"/>
     </row>
     <row r="160" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B160" s="13"/>
-      <c r="C160" s="13"/>
       <c r="D160" s="13"/>
       <c r="E160" s="12"/>
       <c r="F160" s="1"/>
     </row>
     <row r="161" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B161" s="13"/>
-      <c r="C161" s="13"/>
       <c r="D161" s="13"/>
       <c r="E161" s="12"/>
       <c r="F161" s="1"/>
     </row>
     <row r="162" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B162" s="13"/>
-      <c r="C162" s="13"/>
       <c r="D162" s="13"/>
       <c r="E162" s="12"/>
       <c r="F162" s="1"/>
     </row>
     <row r="163" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B163" s="13"/>
-      <c r="C163" s="13"/>
       <c r="D163" s="13"/>
       <c r="E163" s="12"/>
       <c r="F163" s="1"/>
     </row>
     <row r="164" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B164" s="13"/>
-      <c r="C164" s="13"/>
       <c r="D164" s="13"/>
       <c r="E164" s="12"/>
       <c r="F164" s="1"/>
     </row>
     <row r="165" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B165" s="13"/>
-      <c r="C165" s="13"/>
       <c r="D165" s="13"/>
       <c r="E165" s="12"/>
       <c r="F165" s="1"/>
     </row>
     <row r="166" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B166" s="13"/>
-      <c r="C166" s="13"/>
       <c r="D166" s="13"/>
       <c r="E166" s="12"/>
       <c r="F166" s="1"/>
     </row>
     <row r="167" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B167" s="13"/>
-      <c r="C167" s="13"/>
       <c r="D167" s="13"/>
       <c r="E167" s="12"/>
       <c r="F167" s="1"/>
     </row>
     <row r="168" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B168" s="13"/>
-      <c r="C168" s="13"/>
       <c r="D168" s="13"/>
       <c r="E168" s="12"/>
       <c r="F168" s="1"/>
     </row>
     <row r="169" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B169" s="13"/>
-      <c r="C169" s="13"/>
       <c r="D169" s="13"/>
       <c r="E169" s="12"/>
       <c r="F169" s="1"/>
     </row>
     <row r="170" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B170" s="13"/>
-      <c r="C170" s="13"/>
       <c r="D170" s="13"/>
       <c r="E170" s="12"/>
       <c r="F170" s="1"/>
@@ -2947,22 +2824,17 @@
       <c r="F387" s="1"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation operator="equal" allowBlank="1" showErrorMessage="1" sqref="B11:B12 C12:D12" xr:uid="{31957DAA-6AEB-B34B-A86D-83EFCF2B93E5}">
+  <dataValidations count="2">
+    <dataValidation operator="equal" allowBlank="1" showErrorMessage="1" sqref="B11:B12 D12" xr:uid="{31957DAA-6AEB-B34B-A86D-83EFCF2B93E5}">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
+    <dataValidation operator="equal" allowBlank="1" showErrorMessage="1" sqref="D11" xr:uid="{B462C7C6-4C2B-9B43-9152-3669491B3E1E}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{12EDD063-342B-1F45-AA5F-E11E385D02A7}">
-          <x14:formula1>
-            <xm:f>'/Users/sballesteros/Documents/Freezeman/freezeman/backend/fms_core/static/submission_templates/[Library_preparation_v3_8_0.xlsx]Index'!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>H12:H384</xm:sqref>
-        </x14:dataValidation>
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
         <x14:dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" xr:uid="{99E852CC-97D8-B840-A664-9B2E84BC626A}">
           <x14:formula1>
             <xm:f>Index!$B$2:$B$7</xm:f>
@@ -2979,13 +2851,13 @@
           <x14:formula1>
             <xm:f>Index!$D$2:$D$8</xm:f>
           </x14:formula1>
-          <xm:sqref>H11</xm:sqref>
+          <xm:sqref>H11:H384</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" xr:uid="{ACBAF0F5-63F3-F54E-859F-4E88243D5B57}">
           <x14:formula1>
             <xm:f>Index!$A$2:$A$2</xm:f>
           </x14:formula1>
-          <xm:sqref>C11:D11</xm:sqref>
+          <xm:sqref>C11:C384</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2997,7 +2869,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D07BE83E-81BB-7B4B-B20C-1C27C9CCE468}">
   <dimension ref="A1:O484"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -9356,20 +9228,17 @@
           </x14:formula2>
           <xm:sqref>C9:C104</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" xr:uid="{7D4664FF-ADC3-1B4C-8DD6-3CDA9717828E}">
-          <x14:formula1>
-            <xm:f>'/Users/sballesteros/Documents/Freezeman/Templates/[Library_preparation_v3_8_0.xlsx]Library Batch'!#REF!</xm:f>
-          </x14:formula1>
-          <x14:formula2>
-            <xm:f>0</xm:f>
-          </x14:formula2>
-          <xm:sqref>A8:A103</xm:sqref>
-        </x14:dataValidation>
         <x14:dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" xr:uid="{AC8952C2-1C72-F247-A4E5-E9CC9DC1954B}">
           <x14:formula1>
             <xm:f>Index!$E$2:$E$11</xm:f>
           </x14:formula1>
           <xm:sqref>G8</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" xr:uid="{43B227F3-4B91-7941-A9E4-3E8690FF24F3}">
+          <x14:formula1>
+            <xm:f>'Conversion Batch'!$A$11:$A$384</xm:f>
+          </x14:formula1>
+          <xm:sqref>A8:A384</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>